<commit_message>
Final commit of X
</commit_message>
<xml_diff>
--- a/X/meritve.xlsx
+++ b/X/meritve.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>U_s</t>
   </si>
@@ -46,6 +46,48 @@
   </si>
   <si>
     <t>delta</t>
+  </si>
+  <si>
+    <t>eta</t>
+  </si>
+  <si>
+    <t>0.017</t>
+  </si>
+  <si>
+    <t>0.001 circa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rho </t>
+  </si>
+  <si>
+    <t>at</t>
+  </si>
+  <si>
+    <t>101kPa</t>
+  </si>
+  <si>
+    <t>24C</t>
+  </si>
+  <si>
+    <t>40% rel vla</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>1,17 kgm-3</t>
+  </si>
+  <si>
+    <t>m3</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>2.18E-09</t>
+  </si>
+  <si>
+    <t>3.36E-09</t>
   </si>
 </sst>
 </file>
@@ -82,8 +124,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -364,15 +407,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:J26"/>
+  <dimension ref="C2:Q32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>0</v>
       </c>
@@ -392,7 +435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>0.9</v>
       </c>
@@ -412,7 +455,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>1.7</v>
       </c>
@@ -432,7 +475,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>6.6</v>
       </c>
@@ -452,7 +495,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>7.7</v>
       </c>
@@ -472,7 +515,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>14.4</v>
       </c>
@@ -491,8 +534,14 @@
       <c r="J7">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="O7" t="s">
+        <v>10</v>
+      </c>
+      <c r="P7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>17.2</v>
       </c>
@@ -511,8 +560,11 @@
       <c r="J8">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="O8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>21.4</v>
       </c>
@@ -531,8 +583,11 @@
       <c r="J9">
         <v>0.92</v>
       </c>
-    </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="O9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>26</v>
       </c>
@@ -551,8 +606,11 @@
       <c r="J10">
         <v>1.36</v>
       </c>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="O10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>31.7</v>
       </c>
@@ -571,8 +629,11 @@
       <c r="J11">
         <v>1.57</v>
       </c>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="O11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>34.700000000000003</v>
       </c>
@@ -592,7 +653,7 @@
         <v>1.87</v>
       </c>
     </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>46.4</v>
       </c>
@@ -611,8 +672,17 @@
       <c r="J13">
         <v>2.12</v>
       </c>
-    </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="O13" t="s">
+        <v>15</v>
+      </c>
+      <c r="P13">
+        <v>6.3000000000000003E-4</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>49.5</v>
       </c>
@@ -632,7 +702,7 @@
         <v>2.2799999999999998</v>
       </c>
     </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>57.8</v>
       </c>
@@ -652,7 +722,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>64.2</v>
       </c>
@@ -800,17 +870,32 @@
         <v>3.5</v>
       </c>
     </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C32" s="1">
+        <v>1.1800000000000001E-9</v>
+      </c>
+      <c r="D32" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" t="s">
+        <v>19</v>
+      </c>
+      <c r="I32" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D1:P8"/>
+  <dimension ref="D1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,14 +1137,60 @@
         <v>0.39</v>
       </c>
       <c r="N8">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="O8">
         <f>AVERAGE(O3:O7)</f>
         <v>0.48799999999999999</v>
       </c>
       <c r="P8">
-        <v>0.1</v>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="9" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>121</v>
+      </c>
+      <c r="G9">
+        <v>138</v>
+      </c>
+      <c r="M9">
+        <v>0.39</v>
+      </c>
+      <c r="O9">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="11" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11">
+        <f>(G8-E8)/(E8+G8)</f>
+        <v>6.729916309923252E-2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11" t="s">
+        <v>7</v>
+      </c>
+      <c r="M11">
+        <f>(O8-M8)/(M8+O8)</f>
+        <v>0.11161731207289291</v>
+      </c>
+      <c r="N11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <f>(G9-E9)/(E9+G9)</f>
+        <v>6.5637065637065631E-2</v>
+      </c>
+      <c r="M12">
+        <f>(O9-M9)/(M9+O9)</f>
+        <v>0.1136363636363636</v>
       </c>
     </row>
   </sheetData>

</xml_diff>